<commit_message>
did like one figure lol
</commit_message>
<xml_diff>
--- a/190502_buck_cutoff.xlsx
+++ b/190502_buck_cutoff.xlsx
@@ -5116,9 +5116,9 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
       <sheetData sheetId="4">
         <row r="4">
           <cell r="B4">
@@ -5374,7 +5374,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="5"/>
+      <sheetData sheetId="5" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>

</xml_diff>